<commit_message>
changed a bit of code
</commit_message>
<xml_diff>
--- a/docs/tests/tests.xlsx
+++ b/docs/tests/tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karim\IdeaProjects\homework1softwaredev\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karim\IdeaProjects\homework1softwaredev\docs\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6681F62-AEE6-4128-933B-F610B42249B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81453126-7CE6-4461-9DD1-DDB69C41D367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="14976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Test ID</t>
   </si>
@@ -75,9 +75,6 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <t>Program terminates immediately.</t>
   </si>
   <si>
     <t>TC-02</t>
@@ -305,9 +302,6 @@
     <t>Summarized Output</t>
   </si>
   <si>
-    <t>Treated as incorrect and restarts puzzle with count = 1.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Program treats this as </t>
     </r>
@@ -335,9 +329,6 @@
     <t>Program prints "Your three guesses were wrong" and terminates.</t>
   </si>
   <si>
-    <t>Program prints: "Your guess was: Two and the word was Two" and terminates.</t>
-  </si>
-  <si>
     <t>Prints "Your guess was: unfair and the word was fair". Then prints a new puzzle.</t>
   </si>
   <si>
@@ -348,6 +339,12 @@
   </si>
   <si>
     <t>Commas and periods are not included in the word.</t>
+  </si>
+  <si>
+    <t>Program prints: "Your guess was: Two and the word was Two" and increases correct count by 1.</t>
+  </si>
+  <si>
+    <t>Treated as incorrect and restarts puzzle with incorrectCount += 1.</t>
   </si>
 </sst>
 </file>
@@ -477,15 +474,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
@@ -493,15 +481,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -512,6 +491,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,7 +793,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -825,253 +822,239 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="27.6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>45</v>
+      <c r="F2" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="15"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="18"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="4" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" ht="27.6">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="19"/>
-    </row>
-    <row r="5" spans="1:6" ht="27.6">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:6" ht="28.2" thickBot="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="27.6" customHeight="1">
+      <c r="A8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="19"/>
-    </row>
-    <row r="8" spans="1:6" ht="27.6" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="17" t="s">
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" ht="81" customHeight="1">
+      <c r="A11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:6" ht="28.2" thickBot="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="19"/>
-    </row>
-    <row r="11" spans="1:6" ht="81" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="11" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="12"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+        <v>24</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="28.2" thickBot="1">
       <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.2" thickBot="1">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="42" thickBot="1">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="F17" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="42" thickBot="1">
       <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="F18" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="F11:F15"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -1080,6 +1063,18 @@
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="D5:D7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F8:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>